<commit_message>
Hide time trends and increment version
</commit_message>
<xml_diff>
--- a/inputs/es/Optima_template.xlsx
+++ b/inputs/es/Optima_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominic.delport\Documents\GitHub\Nutrition\inputs\es\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\GitHub\Nutrition\inputs\es\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE689F92-8789-47E2-A866-4F474070794D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B7D8BC-DE01-4965-850A-ACEFC2B3214E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15225" yWindow="-18120" windowWidth="29040" windowHeight="17640" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entradas de población-año base" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Causas de muerte" sheetId="3" r:id="rId3"/>
     <sheet name="Distribución estado nutricional" sheetId="4" r:id="rId4"/>
     <sheet name="Distribución de lactancia" sheetId="5" r:id="rId5"/>
-    <sheet name="Tendencias temporales" sheetId="6" r:id="rId6"/>
+    <sheet name="Tendencias temporales" sheetId="6" state="hidden" r:id="rId6"/>
     <sheet name="Pérdida económica" sheetId="7" r:id="rId7"/>
     <sheet name="Paquetes de IYCF" sheetId="8" r:id="rId8"/>
     <sheet name="Tratamiento de la MAS" sheetId="9" r:id="rId9"/>
@@ -96,8 +96,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -406,7 +410,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="341">
   <si>
     <t>Field</t>
   </si>
@@ -1928,17 +1932,17 @@
     <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="9" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
@@ -2306,19 +2310,19 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6328125" style="98" customWidth="1"/>
-    <col min="2" max="2" width="38.6328125" style="66" customWidth="1"/>
-    <col min="3" max="7" width="14.453125" style="98" customWidth="1"/>
-    <col min="8" max="16384" width="14.453125" style="98"/>
+    <col min="1" max="1" width="27.6640625" style="98" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" style="66" customWidth="1"/>
+    <col min="3" max="7" width="14.44140625" style="98" customWidth="1"/>
+    <col min="8" max="16384" width="14.44140625" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
         <v>19</v>
       </c>
@@ -2329,14 +2333,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="98" t="s">
         <v>55</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
     </row>
-    <row r="3" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="71"/>
       <c r="B3" s="70" t="s">
         <v>18</v>
@@ -2345,7 +2349,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
       <c r="B4" s="70" t="s">
         <v>26</v>
@@ -2354,7 +2358,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -2409,7 +2413,7 @@
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="98"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="98" t="s">
         <v>28</v>
       </c>
@@ -2444,7 +2448,7 @@
       <c r="B20" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="102">
+      <c r="C20" s="100">
         <f>1-frac_rice-frac_wheat-frac_maize</f>
         <v>1</v>
       </c>
@@ -2516,17 +2520,17 @@
       </c>
       <c r="C32" s="43"/>
     </row>
-    <row r="33" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="103">
+      <c r="C33" s="101">
         <f>SUM(C29:C32)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="53" t="s">
         <v>20</v>
       </c>
@@ -2612,7 +2616,7 @@
       <c r="B48" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="102">
+      <c r="C48" s="100">
         <f>1-preterm_SGA-preterm_AGA-term_SGA</f>
         <v>1</v>
       </c>
@@ -2694,7 +2698,7 @@
       </c>
       <c r="C62" s="33"/>
     </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="53"/>
     </row>
   </sheetData>
@@ -2716,20 +2720,20 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" style="70" customWidth="1"/>
     <col min="2" max="2" width="20" style="98" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" style="98" customWidth="1"/>
-    <col min="4" max="4" width="20.08984375" style="98" customWidth="1"/>
-    <col min="5" max="5" width="36.36328125" style="98" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="98" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="98" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" style="98" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="98" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.6328125" style="98" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="14.453125" style="98" customWidth="1"/>
-    <col min="13" max="16384" width="14.453125" style="98"/>
+    <col min="7" max="7" width="22.6640625" style="98" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="14.44140625" style="98" customWidth="1"/>
+    <col min="13" max="16384" width="14.44140625" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
         <v>163</v>
       </c>
@@ -3494,16 +3498,16 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" style="70" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.90625" style="98" customWidth="1"/>
-    <col min="3" max="3" width="42.453125" style="98" customWidth="1"/>
-    <col min="4" max="8" width="11.453125" style="98" customWidth="1"/>
-    <col min="9" max="16384" width="11.453125" style="98"/>
+    <col min="2" max="2" width="47.88671875" style="98" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" style="98" customWidth="1"/>
+    <col min="4" max="8" width="11.44140625" style="98" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>163</v>
       </c>
@@ -3644,14 +3648,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.08984375" style="98" customWidth="1"/>
-    <col min="2" max="6" width="11.453125" style="98" customWidth="1"/>
-    <col min="7" max="16384" width="11.453125" style="98"/>
+    <col min="1" max="1" width="30.109375" style="98" customWidth="1"/>
+    <col min="2" max="6" width="11.44140625" style="98" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>163</v>
       </c>
@@ -3744,7 +3748,7 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="79" t="s">
@@ -3859,19 +3863,19 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.90625" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>209</v>
       </c>
@@ -3918,7 +3922,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>83</v>
       </c>
@@ -4479,7 +4483,7 @@
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
         <v>104</v>
       </c>
@@ -4530,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="53"/>
       <c r="B16" s="70" t="s">
         <v>166</v>
@@ -4575,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
       <c r="B17" s="70" t="s">
         <v>178</v>
@@ -4624,7 +4628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="53"/>
       <c r="B18" s="70" t="s">
         <v>179</v>
@@ -4860,7 +4864,7 @@
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="18"/>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="53" t="s">
         <v>211</v>
       </c>
@@ -5110,7 +5114,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="53" t="s">
         <v>210</v>
       </c>
@@ -5615,7 +5619,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="98" t="s">
@@ -5654,17 +5658,17 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.6328125" style="98" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" style="98" customWidth="1"/>
-    <col min="3" max="4" width="11.453125" style="98" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="98" customWidth="1"/>
-    <col min="6" max="10" width="11.453125" style="98" customWidth="1"/>
-    <col min="11" max="16384" width="11.453125" style="98"/>
+    <col min="1" max="1" width="33.6640625" style="98" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="98" customWidth="1"/>
+    <col min="3" max="4" width="11.44140625" style="98" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="98" customWidth="1"/>
+    <col min="6" max="10" width="11.44140625" style="98" customWidth="1"/>
+    <col min="11" max="16384" width="11.44140625" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>223</v>
       </c>
@@ -5681,7 +5685,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>215</v>
       </c>
@@ -5699,7 +5703,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>222</v>
       </c>
@@ -5717,7 +5721,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>217</v>
       </c>
@@ -5735,7 +5739,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>221</v>
       </c>
@@ -5753,7 +5757,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>220</v>
       </c>
@@ -5771,7 +5775,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>224</v>
       </c>
@@ -5789,7 +5793,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>226</v>
       </c>
@@ -5807,7 +5811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>218</v>
       </c>
@@ -5825,7 +5829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>219</v>
       </c>
@@ -5862,21 +5866,21 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.1796875" style="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.90625" style="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" style="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" style="52" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" style="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="52" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.08984375" style="52" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="15.36328125" style="52" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="16.90625" style="52" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="16.08984375" style="52" customWidth="1"/>
-    <col min="21" max="16384" width="16.08984375" style="52"/>
+    <col min="6" max="7" width="13.109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="15.33203125" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="16.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="16.109375" style="52" customWidth="1"/>
+    <col min="21" max="16384" width="16.109375" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="53" t="s">
         <v>209</v>
       </c>
@@ -5923,7 +5927,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53" t="s">
         <v>83</v>
       </c>
@@ -5970,7 +5974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="70" t="s">
         <v>169</v>
       </c>
@@ -6014,7 +6018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="70" t="s">
         <v>151</v>
       </c>
@@ -6058,7 +6062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="70" t="s">
         <v>152</v>
       </c>
@@ -6102,7 +6106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="70" t="s">
         <v>153</v>
       </c>
@@ -6146,7 +6150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="70" t="s">
         <v>182</v>
       </c>
@@ -6190,7 +6194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="70" t="s">
         <v>184</v>
       </c>
@@ -6234,7 +6238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="70" t="s">
         <v>190</v>
       </c>
@@ -6278,7 +6282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="70" t="s">
         <v>192</v>
       </c>
@@ -6322,7 +6326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="70" t="s">
         <v>193</v>
       </c>
@@ -6366,7 +6370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="70" t="s">
         <v>204</v>
       </c>
@@ -6410,7 +6414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="70" t="s">
         <v>164</v>
       </c>
@@ -6454,7 +6458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="70" t="s">
         <v>196</v>
       </c>
@@ -6498,7 +6502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="70" t="s">
         <v>202</v>
       </c>
@@ -6542,7 +6546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="70" t="s">
         <v>203</v>
       </c>
@@ -6586,7 +6590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="70"/>
       <c r="C17" s="80"/>
       <c r="D17" s="80"/>
@@ -6602,7 +6606,7 @@
       <c r="N17" s="80"/>
       <c r="O17" s="80"/>
     </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="53" t="s">
         <v>104</v>
       </c>
@@ -6649,7 +6653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="53"/>
       <c r="B19" s="70" t="s">
         <v>166</v>
@@ -6694,7 +6698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="70" t="s">
         <v>178</v>
       </c>
@@ -6738,7 +6742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="70" t="s">
         <v>179</v>
       </c>
@@ -6782,7 +6786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="50" t="s">
         <v>180</v>
       </c>
@@ -6826,7 +6830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="70" t="s">
         <v>188</v>
       </c>
@@ -6870,7 +6874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="70" t="s">
         <v>189</v>
       </c>
@@ -6914,7 +6918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="70" t="s">
         <v>191</v>
       </c>
@@ -6958,7 +6962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="70"/>
       <c r="C26" s="80"/>
       <c r="D26" s="80"/>
@@ -6974,7 +6978,7 @@
       <c r="N26" s="80"/>
       <c r="O26" s="80"/>
     </row>
-    <row r="27" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="53" t="s">
         <v>211</v>
       </c>
@@ -7022,7 +7026,7 @@
       </c>
       <c r="P27" s="51"/>
     </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="66" t="s">
         <v>174</v>
       </c>
@@ -7066,7 +7070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="53"/>
       <c r="B29" s="66" t="s">
         <v>175</v>
@@ -7111,7 +7115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="66" t="s">
         <v>176</v>
       </c>
@@ -7155,7 +7159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="66" t="s">
         <v>177</v>
       </c>
@@ -7199,7 +7203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="70"/>
       <c r="C32" s="81"/>
       <c r="D32" s="81"/>
@@ -7215,7 +7219,7 @@
       <c r="N32" s="80"/>
       <c r="O32" s="80"/>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="53" t="s">
         <v>210</v>
       </c>
@@ -7262,7 +7266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="70" t="s">
         <v>172</v>
       </c>
@@ -7306,7 +7310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="70" t="s">
         <v>173</v>
       </c>
@@ -7350,7 +7354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="70" t="s">
         <v>181</v>
       </c>
@@ -7394,7 +7398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="70" t="s">
         <v>185</v>
       </c>
@@ -7438,7 +7442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="70" t="s">
         <v>197</v>
       </c>
@@ -7482,7 +7486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="70" t="s">
         <v>198</v>
       </c>
@@ -7526,7 +7530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="70" t="s">
         <v>199</v>
       </c>
@@ -7570,7 +7574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="70" t="s">
         <v>200</v>
       </c>
@@ -7614,7 +7618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="70" t="s">
         <v>201</v>
       </c>
@@ -7675,23 +7679,23 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.90625" style="98" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" style="98" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" style="98" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" style="98" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="98" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="98" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="98" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.90625" style="98" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" style="98" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.36328125" style="98" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="12.81640625" style="98" customWidth="1"/>
-    <col min="16" max="16384" width="12.81640625" style="98"/>
+    <col min="1" max="1" width="58.88671875" style="98" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="98" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="98" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="98" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="98" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="98" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" style="98" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="98" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="98" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="98" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="12.77734375" style="98" customWidth="1"/>
+    <col min="16" max="16384" width="12.77734375" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>163</v>
       </c>
@@ -8443,23 +8447,23 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.90625" style="98" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" style="98" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" style="98" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" style="98" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="98" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="98" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="98" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.90625" style="98" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" style="98" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.36328125" style="98" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="12.81640625" style="98" customWidth="1"/>
-    <col min="16" max="16384" width="12.81640625" style="98"/>
+    <col min="1" max="1" width="16.88671875" style="98" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="98" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="98" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="98" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="98" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="98" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" style="98" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="98" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="98" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="98" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="12.77734375" style="98" customWidth="1"/>
+    <col min="16" max="16384" width="12.77734375" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>233</v>
       </c>
@@ -8818,15 +8822,15 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.453125" style="98" customWidth="1"/>
-    <col min="2" max="9" width="16.90625" style="98" customWidth="1"/>
-    <col min="10" max="14" width="14.453125" style="98" customWidth="1"/>
-    <col min="15" max="16384" width="14.453125" style="98"/>
+    <col min="1" max="1" width="8.44140625" style="98" customWidth="1"/>
+    <col min="2" max="9" width="16.88671875" style="98" customWidth="1"/>
+    <col min="10" max="14" width="14.44140625" style="98" customWidth="1"/>
+    <col min="15" max="16384" width="14.44140625" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
         <v>73</v>
       </c>
@@ -9814,16 +9818,16 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.08984375" style="98" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" style="98" customWidth="1"/>
     <col min="2" max="2" width="15" style="98" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" style="98" customWidth="1"/>
-    <col min="4" max="8" width="12.81640625" style="98" customWidth="1"/>
-    <col min="9" max="16384" width="12.81640625" style="98"/>
+    <col min="3" max="3" width="14.6640625" style="98" customWidth="1"/>
+    <col min="4" max="8" width="12.77734375" style="98" customWidth="1"/>
+    <col min="9" max="16384" width="12.77734375" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>234</v>
       </c>
@@ -9849,11 +9853,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>236</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="103" t="s">
         <v>104</v>
       </c>
       <c r="C2" s="98" t="s">
@@ -9876,7 +9880,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="101"/>
+      <c r="B3" s="104"/>
       <c r="C3" s="98" t="s">
         <v>149</v>
       </c>
@@ -9898,7 +9902,7 @@
       <c r="J3" s="54"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="101"/>
+      <c r="B4" s="104"/>
       <c r="C4" s="98" t="s">
         <v>155</v>
       </c>
@@ -9920,7 +9924,7 @@
       <c r="J4" s="54"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="103" t="s">
         <v>78</v>
       </c>
       <c r="C5" s="98" t="s">
@@ -9944,7 +9948,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="101"/>
+      <c r="B6" s="104"/>
       <c r="C6" s="98" t="s">
         <v>149</v>
       </c>
@@ -9965,7 +9969,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="101"/>
+      <c r="B7" s="104"/>
       <c r="C7" s="98" t="s">
         <v>155</v>
       </c>
@@ -9986,7 +9990,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="103" t="s">
         <v>74</v>
       </c>
       <c r="C8" s="98" t="s">
@@ -10009,7 +10013,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="101"/>
+      <c r="B9" s="104"/>
       <c r="C9" s="98" t="s">
         <v>149</v>
       </c>
@@ -10030,7 +10034,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="101"/>
+      <c r="B10" s="104"/>
       <c r="C10" s="98" t="s">
         <v>155</v>
       </c>
@@ -10051,7 +10055,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="100" t="s">
+      <c r="B11" s="103" t="s">
         <v>77</v>
       </c>
       <c r="C11" s="98" t="s">
@@ -10074,7 +10078,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="101"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="98" t="s">
         <v>149</v>
       </c>
@@ -10095,7 +10099,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="101"/>
+      <c r="B13" s="104"/>
       <c r="C13" s="98" t="s">
         <v>155</v>
       </c>
@@ -10116,7 +10120,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="100" t="s">
+      <c r="B14" s="103" t="s">
         <v>75</v>
       </c>
       <c r="C14" s="98" t="s">
@@ -10139,7 +10143,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="101"/>
+      <c r="B15" s="104"/>
       <c r="C15" s="98" t="s">
         <v>149</v>
       </c>
@@ -10160,7 +10164,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="101"/>
+      <c r="B16" s="104"/>
       <c r="C16" s="98" t="s">
         <v>155</v>
       </c>
@@ -10180,7 +10184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="97" t="s">
         <v>148</v>
       </c>
@@ -10210,11 +10214,11 @@
       <c r="G18" s="82"/>
       <c r="H18" s="82"/>
     </row>
-    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="53" t="s">
         <v>242</v>
       </c>
-      <c r="B19" s="100" t="s">
+      <c r="B19" s="103" t="s">
         <v>104</v>
       </c>
       <c r="C19" s="98" t="s">
@@ -10237,7 +10241,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="101"/>
+      <c r="B20" s="104"/>
       <c r="C20" s="98" t="s">
         <v>149</v>
       </c>
@@ -10258,7 +10262,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="101"/>
+      <c r="B21" s="104"/>
       <c r="C21" s="98" t="s">
         <v>155</v>
       </c>
@@ -10279,7 +10283,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="100" t="s">
+      <c r="B22" s="103" t="s">
         <v>78</v>
       </c>
       <c r="C22" s="98" t="s">
@@ -10302,7 +10306,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="101"/>
+      <c r="B23" s="104"/>
       <c r="C23" s="98" t="s">
         <v>149</v>
       </c>
@@ -10323,7 +10327,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="101"/>
+      <c r="B24" s="104"/>
       <c r="C24" s="98" t="s">
         <v>155</v>
       </c>
@@ -10344,7 +10348,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="100" t="s">
+      <c r="B25" s="103" t="s">
         <v>74</v>
       </c>
       <c r="C25" s="98" t="s">
@@ -10367,7 +10371,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="101"/>
+      <c r="B26" s="104"/>
       <c r="C26" s="98" t="s">
         <v>149</v>
       </c>
@@ -10388,7 +10392,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="101"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="98" t="s">
         <v>155</v>
       </c>
@@ -10409,7 +10413,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="100" t="s">
+      <c r="B28" s="103" t="s">
         <v>77</v>
       </c>
       <c r="C28" s="98" t="s">
@@ -10432,7 +10436,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="101"/>
+      <c r="B29" s="104"/>
       <c r="C29" s="98" t="s">
         <v>149</v>
       </c>
@@ -10453,7 +10457,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="101"/>
+      <c r="B30" s="104"/>
       <c r="C30" s="98" t="s">
         <v>155</v>
       </c>
@@ -10474,7 +10478,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="100" t="s">
+      <c r="B31" s="103" t="s">
         <v>75</v>
       </c>
       <c r="C31" s="98" t="s">
@@ -10497,7 +10501,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="101"/>
+      <c r="B32" s="104"/>
       <c r="C32" s="98" t="s">
         <v>149</v>
       </c>
@@ -10518,7 +10522,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="101"/>
+      <c r="B33" s="104"/>
       <c r="C33" s="98" t="s">
         <v>155</v>
       </c>
@@ -10538,7 +10542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="97" t="s">
         <v>148</v>
       </c>
@@ -10568,11 +10572,11 @@
       <c r="G35" s="82"/>
       <c r="H35" s="82"/>
     </row>
-    <row r="36" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="55" t="s">
         <v>239</v>
       </c>
-      <c r="B36" s="100" t="s">
+      <c r="B36" s="103" t="s">
         <v>104</v>
       </c>
       <c r="C36" s="98" t="s">
@@ -10595,7 +10599,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="101"/>
+      <c r="B37" s="104"/>
       <c r="C37" s="98" t="s">
         <v>149</v>
       </c>
@@ -10616,7 +10620,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="101"/>
+      <c r="B38" s="104"/>
       <c r="C38" s="98" t="s">
         <v>155</v>
       </c>
@@ -10637,7 +10641,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="100" t="s">
+      <c r="B39" s="103" t="s">
         <v>78</v>
       </c>
       <c r="C39" s="98" t="s">
@@ -10660,7 +10664,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="101"/>
+      <c r="B40" s="104"/>
       <c r="C40" s="98" t="s">
         <v>149</v>
       </c>
@@ -10681,7 +10685,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="101"/>
+      <c r="B41" s="104"/>
       <c r="C41" s="98" t="s">
         <v>155</v>
       </c>
@@ -10702,7 +10706,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="100" t="s">
+      <c r="B42" s="103" t="s">
         <v>74</v>
       </c>
       <c r="C42" s="98" t="s">
@@ -10725,7 +10729,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="101"/>
+      <c r="B43" s="104"/>
       <c r="C43" s="98" t="s">
         <v>149</v>
       </c>
@@ -10746,7 +10750,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="101"/>
+      <c r="B44" s="104"/>
       <c r="C44" s="98" t="s">
         <v>155</v>
       </c>
@@ -10767,7 +10771,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="100" t="s">
+      <c r="B45" s="103" t="s">
         <v>77</v>
       </c>
       <c r="C45" s="98" t="s">
@@ -10790,7 +10794,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="101"/>
+      <c r="B46" s="104"/>
       <c r="C46" s="98" t="s">
         <v>149</v>
       </c>
@@ -10811,7 +10815,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="101"/>
+      <c r="B47" s="104"/>
       <c r="C47" s="98" t="s">
         <v>155</v>
       </c>
@@ -10832,7 +10836,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="100" t="s">
+      <c r="B48" s="103" t="s">
         <v>75</v>
       </c>
       <c r="C48" s="98" t="s">
@@ -10855,7 +10859,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="101"/>
+      <c r="B49" s="104"/>
       <c r="C49" s="98" t="s">
         <v>149</v>
       </c>
@@ -10876,7 +10880,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="101"/>
+      <c r="B50" s="104"/>
       <c r="C50" s="98" t="s">
         <v>155</v>
       </c>
@@ -10896,7 +10900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B51" s="97" t="s">
         <v>148</v>
       </c>
@@ -10919,7 +10923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="89" t="s">
         <v>235</v>
       </c>
@@ -10931,7 +10935,7 @@
       <c r="G53" s="89"/>
       <c r="H53" s="89"/>
     </row>
-    <row r="54" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="53" t="s">
         <v>234</v>
       </c>
@@ -10957,11 +10961,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="B55" s="100" t="s">
+      <c r="B55" s="103" t="s">
         <v>104</v>
       </c>
       <c r="C55" s="98" t="s">
@@ -10989,7 +10993,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="101"/>
+      <c r="B56" s="104"/>
       <c r="C56" s="98" t="s">
         <v>149</v>
       </c>
@@ -11015,7 +11019,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="101"/>
+      <c r="B57" s="104"/>
       <c r="C57" s="98" t="s">
         <v>155</v>
       </c>
@@ -11041,7 +11045,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="100" t="s">
+      <c r="B58" s="103" t="s">
         <v>78</v>
       </c>
       <c r="C58" s="98" t="s">
@@ -11069,7 +11073,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="101"/>
+      <c r="B59" s="104"/>
       <c r="C59" s="98" t="s">
         <v>149</v>
       </c>
@@ -11095,7 +11099,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="101"/>
+      <c r="B60" s="104"/>
       <c r="C60" s="98" t="s">
         <v>155</v>
       </c>
@@ -11121,7 +11125,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="100" t="s">
+      <c r="B61" s="103" t="s">
         <v>74</v>
       </c>
       <c r="C61" s="98" t="s">
@@ -11149,7 +11153,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="101"/>
+      <c r="B62" s="104"/>
       <c r="C62" s="98" t="s">
         <v>149</v>
       </c>
@@ -11175,7 +11179,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="101"/>
+      <c r="B63" s="104"/>
       <c r="C63" s="98" t="s">
         <v>155</v>
       </c>
@@ -11201,7 +11205,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="100" t="s">
+      <c r="B64" s="103" t="s">
         <v>77</v>
       </c>
       <c r="C64" s="98" t="s">
@@ -11229,7 +11233,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="101"/>
+      <c r="B65" s="104"/>
       <c r="C65" s="98" t="s">
         <v>149</v>
       </c>
@@ -11255,7 +11259,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="101"/>
+      <c r="B66" s="104"/>
       <c r="C66" s="98" t="s">
         <v>155</v>
       </c>
@@ -11281,7 +11285,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="100" t="s">
+      <c r="B67" s="103" t="s">
         <v>75</v>
       </c>
       <c r="C67" s="98" t="s">
@@ -11309,7 +11313,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="101"/>
+      <c r="B68" s="104"/>
       <c r="C68" s="98" t="s">
         <v>149</v>
       </c>
@@ -11335,7 +11339,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="101"/>
+      <c r="B69" s="104"/>
       <c r="C69" s="98" t="s">
         <v>155</v>
       </c>
@@ -11360,7 +11364,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" s="97" t="s">
         <v>148</v>
       </c>
@@ -11395,11 +11399,11 @@
       <c r="G71" s="82"/>
       <c r="H71" s="82"/>
     </row>
-    <row r="72" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="53" t="s">
         <v>243</v>
       </c>
-      <c r="B72" s="100" t="s">
+      <c r="B72" s="103" t="s">
         <v>104</v>
       </c>
       <c r="C72" s="98" t="s">
@@ -11427,7 +11431,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B73" s="101"/>
+      <c r="B73" s="104"/>
       <c r="C73" s="98" t="s">
         <v>149</v>
       </c>
@@ -11453,7 +11457,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="101"/>
+      <c r="B74" s="104"/>
       <c r="C74" s="98" t="s">
         <v>155</v>
       </c>
@@ -11479,7 +11483,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="100" t="s">
+      <c r="B75" s="103" t="s">
         <v>78</v>
       </c>
       <c r="C75" s="98" t="s">
@@ -11507,7 +11511,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="101"/>
+      <c r="B76" s="104"/>
       <c r="C76" s="98" t="s">
         <v>149</v>
       </c>
@@ -11533,7 +11537,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="101"/>
+      <c r="B77" s="104"/>
       <c r="C77" s="98" t="s">
         <v>155</v>
       </c>
@@ -11559,7 +11563,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="100" t="s">
+      <c r="B78" s="103" t="s">
         <v>74</v>
       </c>
       <c r="C78" s="98" t="s">
@@ -11587,7 +11591,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="101"/>
+      <c r="B79" s="104"/>
       <c r="C79" s="98" t="s">
         <v>149</v>
       </c>
@@ -11613,7 +11617,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="101"/>
+      <c r="B80" s="104"/>
       <c r="C80" s="98" t="s">
         <v>155</v>
       </c>
@@ -11639,7 +11643,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="100" t="s">
+      <c r="B81" s="103" t="s">
         <v>77</v>
       </c>
       <c r="C81" s="98" t="s">
@@ -11667,7 +11671,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="101"/>
+      <c r="B82" s="104"/>
       <c r="C82" s="98" t="s">
         <v>149</v>
       </c>
@@ -11693,7 +11697,7 @@
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="101"/>
+      <c r="B83" s="104"/>
       <c r="C83" s="98" t="s">
         <v>155</v>
       </c>
@@ -11719,7 +11723,7 @@
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="100" t="s">
+      <c r="B84" s="103" t="s">
         <v>75</v>
       </c>
       <c r="C84" s="98" t="s">
@@ -11747,7 +11751,7 @@
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="101"/>
+      <c r="B85" s="104"/>
       <c r="C85" s="98" t="s">
         <v>149</v>
       </c>
@@ -11773,7 +11777,7 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="101"/>
+      <c r="B86" s="104"/>
       <c r="C86" s="98" t="s">
         <v>155</v>
       </c>
@@ -11798,7 +11802,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B87" s="97" t="s">
         <v>148</v>
       </c>
@@ -11833,11 +11837,11 @@
       <c r="G88" s="82"/>
       <c r="H88" s="82"/>
     </row>
-    <row r="89" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="55" t="s">
         <v>240</v>
       </c>
-      <c r="B89" s="100" t="s">
+      <c r="B89" s="103" t="s">
         <v>104</v>
       </c>
       <c r="C89" s="98" t="s">
@@ -11865,7 +11869,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="101"/>
+      <c r="B90" s="104"/>
       <c r="C90" s="98" t="s">
         <v>149</v>
       </c>
@@ -11891,7 +11895,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="101"/>
+      <c r="B91" s="104"/>
       <c r="C91" s="98" t="s">
         <v>155</v>
       </c>
@@ -11917,7 +11921,7 @@
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="100" t="s">
+      <c r="B92" s="103" t="s">
         <v>78</v>
       </c>
       <c r="C92" s="98" t="s">
@@ -11945,7 +11949,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="101"/>
+      <c r="B93" s="104"/>
       <c r="C93" s="98" t="s">
         <v>149</v>
       </c>
@@ -11971,7 +11975,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="101"/>
+      <c r="B94" s="104"/>
       <c r="C94" s="98" t="s">
         <v>155</v>
       </c>
@@ -11997,7 +12001,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="100" t="s">
+      <c r="B95" s="103" t="s">
         <v>74</v>
       </c>
       <c r="C95" s="98" t="s">
@@ -12025,7 +12029,7 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="101"/>
+      <c r="B96" s="104"/>
       <c r="C96" s="98" t="s">
         <v>149</v>
       </c>
@@ -12051,7 +12055,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B97" s="101"/>
+      <c r="B97" s="104"/>
       <c r="C97" s="98" t="s">
         <v>155</v>
       </c>
@@ -12077,7 +12081,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B98" s="100" t="s">
+      <c r="B98" s="103" t="s">
         <v>77</v>
       </c>
       <c r="C98" s="98" t="s">
@@ -12105,7 +12109,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B99" s="101"/>
+      <c r="B99" s="104"/>
       <c r="C99" s="98" t="s">
         <v>149</v>
       </c>
@@ -12131,7 +12135,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B100" s="101"/>
+      <c r="B100" s="104"/>
       <c r="C100" s="98" t="s">
         <v>155</v>
       </c>
@@ -12157,7 +12161,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B101" s="100" t="s">
+      <c r="B101" s="103" t="s">
         <v>75</v>
       </c>
       <c r="C101" s="98" t="s">
@@ -12185,7 +12189,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B102" s="101"/>
+      <c r="B102" s="104"/>
       <c r="C102" s="98" t="s">
         <v>149</v>
       </c>
@@ -12211,7 +12215,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B103" s="101"/>
+      <c r="B103" s="104"/>
       <c r="C103" s="98" t="s">
         <v>155</v>
       </c>
@@ -12236,7 +12240,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B104" s="97" t="s">
         <v>148</v>
       </c>
@@ -12264,7 +12268,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="89" t="s">
         <v>245</v>
       </c>
@@ -12276,7 +12280,7 @@
       <c r="G106" s="89"/>
       <c r="H106" s="89"/>
     </row>
-    <row r="107" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="53" t="s">
         <v>234</v>
       </c>
@@ -12302,11 +12306,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="53" t="s">
         <v>238</v>
       </c>
-      <c r="B108" s="100" t="s">
+      <c r="B108" s="103" t="s">
         <v>104</v>
       </c>
       <c r="C108" s="98" t="s">
@@ -12334,7 +12338,7 @@
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B109" s="101"/>
+      <c r="B109" s="104"/>
       <c r="C109" s="98" t="s">
         <v>149</v>
       </c>
@@ -12360,7 +12364,7 @@
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B110" s="101"/>
+      <c r="B110" s="104"/>
       <c r="C110" s="98" t="s">
         <v>155</v>
       </c>
@@ -12386,7 +12390,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B111" s="100" t="s">
+      <c r="B111" s="103" t="s">
         <v>78</v>
       </c>
       <c r="C111" s="98" t="s">
@@ -12414,7 +12418,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B112" s="101"/>
+      <c r="B112" s="104"/>
       <c r="C112" s="98" t="s">
         <v>149</v>
       </c>
@@ -12440,7 +12444,7 @@
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B113" s="101"/>
+      <c r="B113" s="104"/>
       <c r="C113" s="98" t="s">
         <v>155</v>
       </c>
@@ -12466,7 +12470,7 @@
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B114" s="100" t="s">
+      <c r="B114" s="103" t="s">
         <v>74</v>
       </c>
       <c r="C114" s="98" t="s">
@@ -12494,7 +12498,7 @@
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B115" s="101"/>
+      <c r="B115" s="104"/>
       <c r="C115" s="98" t="s">
         <v>149</v>
       </c>
@@ -12520,7 +12524,7 @@
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B116" s="101"/>
+      <c r="B116" s="104"/>
       <c r="C116" s="98" t="s">
         <v>155</v>
       </c>
@@ -12546,7 +12550,7 @@
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B117" s="100" t="s">
+      <c r="B117" s="103" t="s">
         <v>77</v>
       </c>
       <c r="C117" s="98" t="s">
@@ -12574,7 +12578,7 @@
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B118" s="101"/>
+      <c r="B118" s="104"/>
       <c r="C118" s="98" t="s">
         <v>149</v>
       </c>
@@ -12600,7 +12604,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B119" s="101"/>
+      <c r="B119" s="104"/>
       <c r="C119" s="98" t="s">
         <v>155</v>
       </c>
@@ -12626,7 +12630,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B120" s="100" t="s">
+      <c r="B120" s="103" t="s">
         <v>75</v>
       </c>
       <c r="C120" s="98" t="s">
@@ -12654,7 +12658,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B121" s="101"/>
+      <c r="B121" s="104"/>
       <c r="C121" s="98" t="s">
         <v>149</v>
       </c>
@@ -12680,7 +12684,7 @@
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B122" s="101"/>
+      <c r="B122" s="104"/>
       <c r="C122" s="98" t="s">
         <v>155</v>
       </c>
@@ -12705,7 +12709,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B123" s="97" t="s">
         <v>148</v>
       </c>
@@ -12740,11 +12744,11 @@
       <c r="G124" s="82"/>
       <c r="H124" s="82"/>
     </row>
-    <row r="125" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="53" t="s">
         <v>244</v>
       </c>
-      <c r="B125" s="100" t="s">
+      <c r="B125" s="103" t="s">
         <v>104</v>
       </c>
       <c r="C125" s="98" t="s">
@@ -12772,7 +12776,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B126" s="101"/>
+      <c r="B126" s="104"/>
       <c r="C126" s="98" t="s">
         <v>149</v>
       </c>
@@ -12798,7 +12802,7 @@
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B127" s="101"/>
+      <c r="B127" s="104"/>
       <c r="C127" s="98" t="s">
         <v>155</v>
       </c>
@@ -12824,7 +12828,7 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B128" s="100" t="s">
+      <c r="B128" s="103" t="s">
         <v>78</v>
       </c>
       <c r="C128" s="98" t="s">
@@ -12852,7 +12856,7 @@
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B129" s="101"/>
+      <c r="B129" s="104"/>
       <c r="C129" s="98" t="s">
         <v>149</v>
       </c>
@@ -12878,7 +12882,7 @@
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B130" s="101"/>
+      <c r="B130" s="104"/>
       <c r="C130" s="98" t="s">
         <v>155</v>
       </c>
@@ -12904,7 +12908,7 @@
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B131" s="100" t="s">
+      <c r="B131" s="103" t="s">
         <v>74</v>
       </c>
       <c r="C131" s="98" t="s">
@@ -12932,7 +12936,7 @@
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B132" s="101"/>
+      <c r="B132" s="104"/>
       <c r="C132" s="98" t="s">
         <v>149</v>
       </c>
@@ -12958,7 +12962,7 @@
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B133" s="101"/>
+      <c r="B133" s="104"/>
       <c r="C133" s="98" t="s">
         <v>155</v>
       </c>
@@ -12984,7 +12988,7 @@
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B134" s="100" t="s">
+      <c r="B134" s="103" t="s">
         <v>77</v>
       </c>
       <c r="C134" s="98" t="s">
@@ -13012,7 +13016,7 @@
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B135" s="101"/>
+      <c r="B135" s="104"/>
       <c r="C135" s="98" t="s">
         <v>149</v>
       </c>
@@ -13038,7 +13042,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B136" s="101"/>
+      <c r="B136" s="104"/>
       <c r="C136" s="98" t="s">
         <v>155</v>
       </c>
@@ -13064,7 +13068,7 @@
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B137" s="100" t="s">
+      <c r="B137" s="103" t="s">
         <v>75</v>
       </c>
       <c r="C137" s="98" t="s">
@@ -13092,7 +13096,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B138" s="101"/>
+      <c r="B138" s="104"/>
       <c r="C138" s="98" t="s">
         <v>149</v>
       </c>
@@ -13118,7 +13122,7 @@
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B139" s="101"/>
+      <c r="B139" s="104"/>
       <c r="C139" s="98" t="s">
         <v>155</v>
       </c>
@@ -13143,7 +13147,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B140" s="97" t="s">
         <v>148</v>
       </c>
@@ -13178,11 +13182,11 @@
       <c r="G141" s="82"/>
       <c r="H141" s="82"/>
     </row>
-    <row r="142" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="55" t="s">
         <v>241</v>
       </c>
-      <c r="B142" s="100" t="s">
+      <c r="B142" s="103" t="s">
         <v>104</v>
       </c>
       <c r="C142" s="98" t="s">
@@ -13210,7 +13214,7 @@
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B143" s="101"/>
+      <c r="B143" s="104"/>
       <c r="C143" s="98" t="s">
         <v>149</v>
       </c>
@@ -13236,7 +13240,7 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B144" s="101"/>
+      <c r="B144" s="104"/>
       <c r="C144" s="98" t="s">
         <v>155</v>
       </c>
@@ -13262,7 +13266,7 @@
       </c>
     </row>
     <row r="145" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B145" s="100" t="s">
+      <c r="B145" s="103" t="s">
         <v>78</v>
       </c>
       <c r="C145" s="98" t="s">
@@ -13290,7 +13294,7 @@
       </c>
     </row>
     <row r="146" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B146" s="101"/>
+      <c r="B146" s="104"/>
       <c r="C146" s="98" t="s">
         <v>149</v>
       </c>
@@ -13316,7 +13320,7 @@
       </c>
     </row>
     <row r="147" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B147" s="101"/>
+      <c r="B147" s="104"/>
       <c r="C147" s="98" t="s">
         <v>155</v>
       </c>
@@ -13342,7 +13346,7 @@
       </c>
     </row>
     <row r="148" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B148" s="100" t="s">
+      <c r="B148" s="103" t="s">
         <v>74</v>
       </c>
       <c r="C148" s="98" t="s">
@@ -13370,7 +13374,7 @@
       </c>
     </row>
     <row r="149" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B149" s="101"/>
+      <c r="B149" s="104"/>
       <c r="C149" s="98" t="s">
         <v>149</v>
       </c>
@@ -13396,7 +13400,7 @@
       </c>
     </row>
     <row r="150" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B150" s="101"/>
+      <c r="B150" s="104"/>
       <c r="C150" s="98" t="s">
         <v>155</v>
       </c>
@@ -13422,7 +13426,7 @@
       </c>
     </row>
     <row r="151" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B151" s="100" t="s">
+      <c r="B151" s="103" t="s">
         <v>77</v>
       </c>
       <c r="C151" s="98" t="s">
@@ -13450,7 +13454,7 @@
       </c>
     </row>
     <row r="152" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B152" s="101"/>
+      <c r="B152" s="104"/>
       <c r="C152" s="98" t="s">
         <v>149</v>
       </c>
@@ -13476,7 +13480,7 @@
       </c>
     </row>
     <row r="153" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B153" s="101"/>
+      <c r="B153" s="104"/>
       <c r="C153" s="98" t="s">
         <v>155</v>
       </c>
@@ -13502,7 +13506,7 @@
       </c>
     </row>
     <row r="154" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B154" s="100" t="s">
+      <c r="B154" s="103" t="s">
         <v>75</v>
       </c>
       <c r="C154" s="98" t="s">
@@ -13530,7 +13534,7 @@
       </c>
     </row>
     <row r="155" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B155" s="101"/>
+      <c r="B155" s="104"/>
       <c r="C155" s="98" t="s">
         <v>149</v>
       </c>
@@ -13556,7 +13560,7 @@
       </c>
     </row>
     <row r="156" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B156" s="101"/>
+      <c r="B156" s="104"/>
       <c r="C156" s="98" t="s">
         <v>155</v>
       </c>
@@ -13581,7 +13585,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="157" spans="2:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B157" s="97" t="s">
         <v>148</v>
       </c>
@@ -13612,6 +13616,42 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="E+xb8SGipTpdVsotnLlVrlIWDO5cvWWgPviGTFSAipqcICJVszWympDQKNOiPF8ybfHn0UV8K1wWQbXYRExDZQ==" saltValue="1CwroKRK7eIPVj7uOECOPw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="45">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="B114:B116"/>
+    <mergeCell ref="B117:B119"/>
+    <mergeCell ref="B120:B122"/>
+    <mergeCell ref="B125:B127"/>
     <mergeCell ref="B145:B147"/>
     <mergeCell ref="B148:B150"/>
     <mergeCell ref="B151:B153"/>
@@ -13621,42 +13661,6 @@
     <mergeCell ref="B134:B136"/>
     <mergeCell ref="B137:B139"/>
     <mergeCell ref="B142:B144"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="B114:B116"/>
-    <mergeCell ref="B117:B119"/>
-    <mergeCell ref="B120:B122"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -13674,23 +13678,23 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.90625" style="98" customWidth="1"/>
-    <col min="2" max="2" width="34.08984375" style="98" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" style="98" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" style="98" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="98" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" style="98" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="98" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="98" customWidth="1"/>
     <col min="5" max="6" width="15" style="98" customWidth="1"/>
-    <col min="7" max="11" width="16.08984375" style="98" customWidth="1"/>
-    <col min="12" max="16384" width="16.08984375" style="98"/>
+    <col min="7" max="11" width="16.109375" style="98" customWidth="1"/>
+    <col min="12" max="16384" width="16.109375" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="65" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="65" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="75"/>
       <c r="C2" s="57" t="s">
         <v>58</v>
@@ -13705,7 +13709,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="53" t="s">
         <v>255</v>
       </c>
@@ -13789,7 +13793,7 @@
       <c r="E8" s="54"/>
       <c r="F8" s="54"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>252</v>
       </c>
@@ -13812,7 +13816,7 @@
       <c r="E10" s="54"/>
       <c r="F10" s="54"/>
     </row>
-    <row r="11" spans="1:6" s="65" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="65" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
         <v>261</v>
       </c>
@@ -13821,7 +13825,7 @@
       <c r="E11" s="64"/>
       <c r="F11" s="64"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>249</v>
       </c>
@@ -13881,7 +13885,7 @@
         <v>4.1900000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="53"/>
       <c r="B16" s="66"/>
       <c r="C16" s="67"/>
@@ -13889,7 +13893,7 @@
       <c r="E16" s="54"/>
       <c r="F16" s="54"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
         <v>258</v>
       </c>
@@ -14038,7 +14042,7 @@
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="66"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="89" t="s">
         <v>235</v>
       </c>
@@ -14048,12 +14052,12 @@
       <c r="E27" s="92"/>
       <c r="F27" s="92"/>
     </row>
-    <row r="28" spans="1:6" s="65" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" s="65" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="56" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="75"/>
       <c r="C29" s="57" t="s">
         <v>58</v>
@@ -14068,7 +14072,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="53" t="s">
         <v>256</v>
       </c>
@@ -14168,7 +14172,7 @@
       <c r="E35" s="54"/>
       <c r="F35" s="54"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="53" t="s">
         <v>253</v>
       </c>
@@ -14189,7 +14193,7 @@
         <v>1.071</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="56" t="s">
         <v>261</v>
       </c>
@@ -14199,7 +14203,7 @@
       <c r="E38" s="64"/>
       <c r="F38" s="64"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="53" t="s">
         <v>250</v>
       </c>
@@ -14271,7 +14275,7 @@
         <v>2.9330000000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="53"/>
       <c r="B43" s="66"/>
       <c r="C43" s="67"/>
@@ -14279,7 +14283,7 @@
       <c r="E43" s="54"/>
       <c r="F43" s="54"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="53" t="s">
         <v>259</v>
       </c>
@@ -14457,7 +14461,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="89" t="s">
         <v>245</v>
       </c>
@@ -14467,12 +14471,12 @@
       <c r="E54" s="92"/>
       <c r="F54" s="92"/>
     </row>
-    <row r="55" spans="1:6" s="65" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" s="65" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="56" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="75"/>
       <c r="C56" s="57" t="s">
         <v>58</v>
@@ -14487,7 +14491,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="53" t="s">
         <v>257</v>
       </c>
@@ -14587,7 +14591,7 @@
       <c r="E62" s="54"/>
       <c r="F62" s="54"/>
     </row>
-    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="53" t="s">
         <v>254</v>
       </c>
@@ -14608,7 +14612,7 @@
         <v>1.9890000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="56" t="s">
         <v>261</v>
       </c>
@@ -14618,7 +14622,7 @@
       <c r="E65" s="64"/>
       <c r="F65" s="64"/>
     </row>
-    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="53" t="s">
         <v>251</v>
       </c>
@@ -14690,7 +14694,7 @@
         <v>5.447000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="53"/>
       <c r="B70" s="66"/>
       <c r="C70" s="67"/>
@@ -14698,7 +14702,7 @@
       <c r="E70" s="54"/>
       <c r="F70" s="54"/>
     </row>
-    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="53" t="s">
         <v>260</v>
       </c>
@@ -14894,24 +14898,24 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" style="98" customWidth="1"/>
-    <col min="2" max="2" width="26.90625" style="98" customWidth="1"/>
-    <col min="3" max="3" width="18.36328125" style="98" customWidth="1"/>
-    <col min="4" max="8" width="14.81640625" style="98" customWidth="1"/>
-    <col min="9" max="12" width="15.36328125" style="98" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="16.90625" style="98" bestFit="1" customWidth="1"/>
-    <col min="17" max="21" width="12.81640625" style="98" customWidth="1"/>
-    <col min="22" max="16384" width="12.81640625" style="98"/>
+    <col min="1" max="1" width="27.21875" style="98" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" style="98" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="98" customWidth="1"/>
+    <col min="4" max="8" width="14.77734375" style="98" customWidth="1"/>
+    <col min="9" max="12" width="15.33203125" style="98" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="16.88671875" style="98" bestFit="1" customWidth="1"/>
+    <col min="17" max="21" width="12.77734375" style="98" customWidth="1"/>
+    <col min="22" max="16384" width="12.77734375" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="65" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="73" t="s">
         <v>230</v>
       </c>
@@ -14945,7 +14949,7 @@
       <c r="O2" s="72"/>
       <c r="P2" s="72"/>
     </row>
-    <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="53"/>
       <c r="B3" s="98" t="s">
         <v>84</v>
@@ -15378,7 +15382,7 @@
       <c r="O17" s="73"/>
       <c r="P17" s="73"/>
     </row>
-    <row r="18" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="79" t="s">
         <v>272</v>
       </c>
@@ -15636,12 +15640,12 @@
       <c r="O26" s="73"/>
       <c r="P26" s="73"/>
     </row>
-    <row r="28" spans="1:16" s="65" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="56" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="73" t="s">
         <v>282</v>
       </c>
@@ -15675,7 +15679,7 @@
       <c r="O29" s="72"/>
       <c r="P29" s="72"/>
     </row>
-    <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="53"/>
       <c r="B30" s="98" t="s">
         <v>84</v>
@@ -16370,12 +16374,12 @@
       <c r="C54" s="79"/>
       <c r="D54" s="79"/>
     </row>
-    <row r="55" spans="1:16" s="65" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="56" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="73" t="s">
         <v>105</v>
       </c>
@@ -16403,7 +16407,7 @@
       <c r="O56" s="72"/>
       <c r="P56" s="72"/>
     </row>
-    <row r="57" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="53"/>
       <c r="B57" s="98" t="s">
         <v>81</v>
@@ -16549,12 +16553,12 @@
       <c r="C63" s="79"/>
       <c r="D63" s="79"/>
     </row>
-    <row r="64" spans="1:16" s="65" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="56" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="73" t="s">
         <v>123</v>
       </c>
@@ -16588,7 +16592,7 @@
       <c r="O65" s="72"/>
       <c r="P65" s="72"/>
     </row>
-    <row r="66" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="77"/>
       <c r="B66" s="98" t="s">
         <v>93</v>
@@ -17624,12 +17628,12 @@
       <c r="O101" s="73"/>
       <c r="P101" s="73"/>
     </row>
-    <row r="103" spans="1:16" s="65" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="56" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="73" t="s">
         <v>84</v>
       </c>
@@ -17663,7 +17667,7 @@
       <c r="O104" s="72"/>
       <c r="P104" s="72"/>
     </row>
-    <row r="105" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="53"/>
       <c r="C105" s="79" t="s">
         <v>124</v>
@@ -17776,13 +17780,13 @@
       <c r="O108" s="73"/>
       <c r="P108" s="73"/>
     </row>
-    <row r="110" spans="1:16" s="90" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" s="90" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="89" t="s">
         <v>235</v>
       </c>
       <c r="H110" s="89"/>
     </row>
-    <row r="111" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="56" t="s">
         <v>278</v>
       </c>
@@ -17794,7 +17798,7 @@
       <c r="G111" s="65"/>
       <c r="H111" s="65"/>
     </row>
-    <row r="112" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="73" t="s">
         <v>230</v>
       </c>
@@ -17820,7 +17824,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="53"/>
       <c r="B113" s="98" t="s">
         <v>84</v>
@@ -18439,7 +18443,7 @@
         <v>2.4079999999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="56" t="s">
         <v>279</v>
       </c>
@@ -18451,7 +18455,7 @@
       <c r="G138" s="65"/>
       <c r="H138" s="65"/>
     </row>
-    <row r="139" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="73" t="s">
         <v>282</v>
       </c>
@@ -18477,7 +18481,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="53"/>
       <c r="B140" s="98" t="s">
         <v>84</v>
@@ -19100,7 +19104,7 @@
       <c r="C164" s="79"/>
       <c r="D164" s="79"/>
     </row>
-    <row r="165" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="56" t="s">
         <v>276</v>
       </c>
@@ -19112,7 +19116,7 @@
       <c r="G165" s="65"/>
       <c r="H165" s="65"/>
     </row>
-    <row r="166" spans="1:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="73" t="s">
         <v>105</v>
       </c>
@@ -19136,7 +19140,7 @@
       </c>
       <c r="H166" s="72"/>
     </row>
-    <row r="167" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="53"/>
       <c r="B167" s="98" t="s">
         <v>81</v>
@@ -19282,7 +19286,7 @@
       <c r="C173" s="79"/>
       <c r="D173" s="79"/>
     </row>
-    <row r="174" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="56" t="s">
         <v>277</v>
       </c>
@@ -19294,7 +19298,7 @@
       <c r="G174" s="65"/>
       <c r="H174" s="65"/>
     </row>
-    <row r="175" spans="1:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="73" t="s">
         <v>123</v>
       </c>
@@ -19320,7 +19324,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="77"/>
       <c r="B176" s="98" t="s">
         <v>93</v>
@@ -20212,7 +20216,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="213" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="56" t="s">
         <v>280</v>
       </c>
@@ -20224,7 +20228,7 @@
       <c r="G213" s="65"/>
       <c r="H213" s="65"/>
     </row>
-    <row r="214" spans="1:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="73" t="s">
         <v>84</v>
       </c>
@@ -20250,7 +20254,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="53"/>
       <c r="C215" s="79" t="s">
         <v>124</v>
@@ -20347,13 +20351,13 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="220" spans="1:9" s="90" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="89" t="s">
         <v>245</v>
       </c>
       <c r="H220" s="89"/>
     </row>
-    <row r="221" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="56" t="s">
         <v>278</v>
       </c>
@@ -20366,7 +20370,7 @@
       <c r="H221" s="65"/>
       <c r="I221" s="65"/>
     </row>
-    <row r="222" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="73" t="s">
         <v>230</v>
       </c>
@@ -20393,7 +20397,7 @@
       </c>
       <c r="I222" s="72"/>
     </row>
-    <row r="223" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="53"/>
       <c r="B223" s="98" t="s">
         <v>84</v>
@@ -21036,7 +21040,7 @@
       </c>
       <c r="I246" s="73"/>
     </row>
-    <row r="248" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" s="56" t="s">
         <v>279</v>
       </c>
@@ -21049,7 +21053,7 @@
       <c r="H248" s="65"/>
       <c r="I248" s="65"/>
     </row>
-    <row r="249" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" s="73" t="s">
         <v>282</v>
       </c>
@@ -21076,7 +21080,7 @@
       </c>
       <c r="I249" s="72"/>
     </row>
-    <row r="250" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" s="53"/>
       <c r="B250" s="98" t="s">
         <v>84</v>
@@ -21723,7 +21727,7 @@
       <c r="C274" s="79"/>
       <c r="D274" s="79"/>
     </row>
-    <row r="275" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" s="56" t="s">
         <v>276</v>
       </c>
@@ -21736,7 +21740,7 @@
       <c r="H275" s="65"/>
       <c r="I275" s="65"/>
     </row>
-    <row r="276" spans="1:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="73" t="s">
         <v>105</v>
       </c>
@@ -21760,7 +21764,7 @@
       </c>
       <c r="H276" s="72"/>
     </row>
-    <row r="277" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" s="53"/>
       <c r="B277" s="98" t="s">
         <v>81</v>
@@ -21906,7 +21910,7 @@
       <c r="C283" s="79"/>
       <c r="D283" s="79"/>
     </row>
-    <row r="284" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" s="56" t="s">
         <v>277</v>
       </c>
@@ -21919,7 +21923,7 @@
       <c r="H284" s="65"/>
       <c r="I284" s="65"/>
     </row>
-    <row r="285" spans="1:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="73" t="s">
         <v>123</v>
       </c>
@@ -21946,7 +21950,7 @@
       </c>
       <c r="I285" s="72"/>
     </row>
-    <row r="286" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" s="77"/>
       <c r="B286" s="98" t="s">
         <v>93</v>
@@ -22874,7 +22878,7 @@
       </c>
       <c r="I321" s="73"/>
     </row>
-    <row r="323" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A323" s="56" t="s">
         <v>280</v>
       </c>
@@ -22887,7 +22891,7 @@
       <c r="H323" s="65"/>
       <c r="I323" s="65"/>
     </row>
-    <row r="324" spans="1:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A324" s="73" t="s">
         <v>84</v>
       </c>
@@ -22914,7 +22918,7 @@
       </c>
       <c r="I324" s="72"/>
     </row>
-    <row r="325" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A325" s="53"/>
       <c r="C325" s="79" t="s">
         <v>124</v>
@@ -23033,25 +23037,25 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.90625" style="98" customWidth="1"/>
-    <col min="2" max="2" width="44.453125" style="98" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" style="98" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" style="98" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" style="98" customWidth="1"/>
+    <col min="1" max="1" width="44.88671875" style="98" customWidth="1"/>
+    <col min="2" max="2" width="44.44140625" style="98" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="98" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="98" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="98" customWidth="1"/>
     <col min="6" max="6" width="15" style="98" customWidth="1"/>
-    <col min="7" max="7" width="13.6328125" style="98" customWidth="1"/>
-    <col min="8" max="12" width="12.81640625" style="98" customWidth="1"/>
-    <col min="13" max="16384" width="12.81640625" style="98"/>
+    <col min="7" max="7" width="13.6640625" style="98" customWidth="1"/>
+    <col min="8" max="12" width="12.77734375" style="98" customWidth="1"/>
+    <col min="13" max="16384" width="12.77734375" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="65" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="65" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>208</v>
       </c>
@@ -23092,7 +23096,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="53"/>
       <c r="B4" s="70" t="s">
         <v>286</v>
@@ -23113,7 +23117,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>283</v>
       </c>
@@ -23206,12 +23210,12 @@
       <c r="F10" s="70"/>
       <c r="G10" s="70"/>
     </row>
-    <row r="11" spans="1:7" s="65" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="65" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="59"/>
       <c r="B12" s="66" t="s">
         <v>182</v>
@@ -23232,16 +23236,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="59"/>
       <c r="B13" s="66"/>
     </row>
-    <row r="14" spans="1:7" s="65" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="65" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="77" t="s">
         <v>282</v>
       </c>
@@ -23264,7 +23268,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="53"/>
       <c r="B16" s="70" t="s">
         <v>291</v>
@@ -23285,7 +23289,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="77" t="s">
         <v>105</v>
       </c>
@@ -23309,12 +23313,12 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:7" s="65" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="65" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="59" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="59" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="53" t="s">
         <v>68</v>
       </c>
@@ -23345,12 +23349,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="89" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="89" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="89" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
         <v>313</v>
       </c>
@@ -23361,7 +23365,7 @@
       <c r="F24" s="65"/>
       <c r="G24" s="65"/>
     </row>
-    <row r="25" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="77" t="s">
         <v>208</v>
       </c>
@@ -23406,7 +23410,7 @@
         <v>157.22999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="53"/>
       <c r="B27" s="70" t="s">
         <v>287</v>
@@ -23432,7 +23436,7 @@
         <v>0.92249999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="59" t="s">
         <v>284</v>
       </c>
@@ -23545,7 +23549,7 @@
       <c r="F33" s="70"/>
       <c r="G33" s="70"/>
     </row>
-    <row r="34" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="56" t="s">
         <v>308</v>
       </c>
@@ -23556,7 +23560,7 @@
       <c r="F34" s="65"/>
       <c r="G34" s="65"/>
     </row>
-    <row r="35" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="59"/>
       <c r="B35" s="66" t="s">
         <v>303</v>
@@ -23579,11 +23583,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="59"/>
       <c r="B36" s="66"/>
     </row>
-    <row r="37" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="56" t="s">
         <v>314</v>
       </c>
@@ -23594,7 +23598,7 @@
       <c r="F37" s="65"/>
       <c r="G37" s="65"/>
     </row>
-    <row r="38" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="77" t="s">
         <v>282</v>
       </c>
@@ -23622,7 +23626,7 @@
         <v>0.92249999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="53"/>
       <c r="B39" s="70" t="s">
         <v>292</v>
@@ -23648,7 +23652,7 @@
         <v>0.92249999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="77" t="s">
         <v>105</v>
       </c>
@@ -23676,7 +23680,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="56" t="s">
         <v>311</v>
       </c>
@@ -23687,7 +23691,7 @@
       <c r="F42" s="65"/>
       <c r="G42" s="65"/>
     </row>
-    <row r="43" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="59"/>
       <c r="B43" s="59"/>
       <c r="C43" s="53" t="s">
@@ -23725,12 +23729,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="89" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" s="89" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="89" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="56" t="s">
         <v>313</v>
       </c>
@@ -23741,7 +23745,7 @@
       <c r="F47" s="65"/>
       <c r="G47" s="65"/>
     </row>
-    <row r="48" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="77" t="s">
         <v>208</v>
       </c>
@@ -23786,7 +23790,7 @@
         <v>183.435</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="53"/>
       <c r="B50" s="70" t="s">
         <v>288</v>
@@ -23812,7 +23816,7 @@
         <v>1.0762499999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="59" t="s">
         <v>285</v>
       </c>
@@ -23925,7 +23929,7 @@
       <c r="F56" s="70"/>
       <c r="G56" s="70"/>
     </row>
-    <row r="57" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="56" t="s">
         <v>309</v>
       </c>
@@ -23936,7 +23940,7 @@
       <c r="F57" s="65"/>
       <c r="G57" s="65"/>
     </row>
-    <row r="58" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="59"/>
       <c r="B58" s="66" t="s">
         <v>304</v>
@@ -23959,11 +23963,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="59"/>
       <c r="B59" s="66"/>
     </row>
-    <row r="60" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="56" t="s">
         <v>314</v>
       </c>
@@ -23974,7 +23978,7 @@
       <c r="F60" s="65"/>
       <c r="G60" s="65"/>
     </row>
-    <row r="61" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="77" t="s">
         <v>282</v>
       </c>
@@ -24002,7 +24006,7 @@
         <v>1.0762499999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="53"/>
       <c r="B62" s="70" t="s">
         <v>293</v>
@@ -24028,7 +24032,7 @@
         <v>1.0762499999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="77" t="s">
         <v>105</v>
       </c>
@@ -24056,7 +24060,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="56" t="s">
         <v>312</v>
       </c>
@@ -24067,7 +24071,7 @@
       <c r="F65" s="65"/>
       <c r="G65" s="65"/>
     </row>
-    <row r="66" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="59"/>
       <c r="B66" s="59"/>
       <c r="C66" s="53" t="s">
@@ -24124,16 +24128,16 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.1796875" style="98" customWidth="1"/>
-    <col min="2" max="6" width="16.08984375" style="98" customWidth="1"/>
-    <col min="7" max="7" width="17.1796875" style="98" customWidth="1"/>
-    <col min="8" max="13" width="16.08984375" style="98" customWidth="1"/>
-    <col min="14" max="16384" width="16.08984375" style="98"/>
+    <col min="1" max="1" width="52.21875" style="98" customWidth="1"/>
+    <col min="2" max="6" width="16.109375" style="98" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" style="98" customWidth="1"/>
+    <col min="8" max="13" width="16.109375" style="98" customWidth="1"/>
+    <col min="14" max="16384" width="16.109375" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
         <v>163</v>
       </c>
@@ -24379,12 +24383,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="89" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="89" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="89" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="71" t="s">
         <v>163</v>
       </c>
@@ -24678,12 +24682,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="89" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="89" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="89" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="71" t="s">
         <v>163</v>
       </c>
@@ -24995,16 +24999,16 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.54296875" style="98" customWidth="1"/>
-    <col min="2" max="2" width="58.90625" style="98" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" style="98" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="98" bestFit="1" customWidth="1"/>
     <col min="3" max="15" width="15" style="98" customWidth="1"/>
-    <col min="16" max="20" width="12.81640625" style="98" customWidth="1"/>
-    <col min="21" max="16384" width="12.81640625" style="98"/>
+    <col min="16" max="20" width="12.77734375" style="98" customWidth="1"/>
+    <col min="21" max="16384" width="12.77734375" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="53"/>
       <c r="B1" s="53"/>
       <c r="C1" s="58" t="s">
@@ -25047,7 +25051,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>326</v>
       </c>
@@ -25492,7 +25496,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="66" t="s">
         <v>190</v>
       </c>
@@ -25624,7 +25628,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
         <v>323</v>
       </c>
@@ -25806,12 +25810,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="89" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" s="89" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="89" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="53"/>
       <c r="B24" s="53"/>
       <c r="C24" s="58" t="s">
@@ -25854,7 +25858,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="53" t="s">
         <v>327</v>
       </c>
@@ -26600,7 +26604,7 @@
         <v>0.29700000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="53" t="s">
         <v>324</v>
       </c>
@@ -26834,12 +26838,12 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="46" spans="1:15" s="89" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" s="89" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="89" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="53"/>
       <c r="B47" s="53"/>
       <c r="C47" s="58" t="s">
@@ -26882,7 +26886,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="53" t="s">
         <v>328</v>
       </c>
@@ -27628,7 +27632,7 @@
         <v>0.34650000000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="53" t="s">
         <v>325</v>
       </c>
@@ -27880,16 +27884,16 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.36328125" style="98" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="98" customWidth="1"/>
-    <col min="3" max="7" width="15.54296875" style="98" customWidth="1"/>
-    <col min="8" max="12" width="12.81640625" style="98" customWidth="1"/>
-    <col min="13" max="16384" width="12.81640625" style="98"/>
+    <col min="1" max="1" width="21.33203125" style="98" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" style="98" customWidth="1"/>
+    <col min="3" max="7" width="15.5546875" style="98" customWidth="1"/>
+    <col min="8" max="12" width="12.77734375" style="98" customWidth="1"/>
+    <col min="13" max="16384" width="12.77734375" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="53"/>
       <c r="B1" s="71"/>
       <c r="C1" s="53" t="s">
@@ -27908,7 +27912,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>333</v>
       </c>
@@ -27933,7 +27937,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="53" t="s">
         <v>330</v>
       </c>
@@ -27964,12 +27968,12 @@
         <v>0.14299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="89" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="89" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="71"/>
       <c r="C8" s="53" t="s">
@@ -27988,7 +27992,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>334</v>
       </c>
@@ -28018,7 +28022,7 @@
         <v>0.189</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>331</v>
       </c>
@@ -28054,12 +28058,12 @@
         <v>0.12869999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="89" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="89" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="89" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="53"/>
       <c r="B15" s="71"/>
       <c r="C15" s="53" t="s">
@@ -28078,7 +28082,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="53" t="s">
         <v>335</v>
       </c>
@@ -28108,7 +28112,7 @@
         <v>0.2205</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="53" t="s">
         <v>332</v>
       </c>
@@ -28162,21 +28166,21 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" style="70" customWidth="1"/>
-    <col min="2" max="2" width="30.54296875" style="70" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" style="70" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" style="70" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" style="70" customWidth="1"/>
     <col min="4" max="4" width="15" style="98" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" style="98" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" style="98" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" style="98" customWidth="1"/>
-    <col min="8" max="8" width="17.54296875" style="98" customWidth="1"/>
-    <col min="9" max="13" width="12.81640625" style="98" customWidth="1"/>
-    <col min="14" max="16384" width="12.81640625" style="98"/>
+    <col min="5" max="5" width="13.6640625" style="98" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="98" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="98" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" style="98" customWidth="1"/>
+    <col min="9" max="13" width="12.77734375" style="98" customWidth="1"/>
+    <col min="14" max="16384" width="12.77734375" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>163</v>
       </c>
@@ -29359,14 +29363,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="90" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="93" t="s">
         <v>329</v>
       </c>
       <c r="B55" s="94"/>
       <c r="C55" s="94"/>
     </row>
-    <row r="56" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="53" t="s">
         <v>163</v>
       </c>
@@ -30809,14 +30813,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" s="90" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="93" t="s">
         <v>336</v>
       </c>
       <c r="B110" s="94"/>
       <c r="C110" s="94"/>
     </row>
-    <row r="111" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="53" t="s">
         <v>163</v>
       </c>
@@ -32277,17 +32281,17 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="98" customWidth="1"/>
-    <col min="2" max="2" width="27.453125" style="98" customWidth="1"/>
-    <col min="3" max="3" width="23.6328125" style="98" customWidth="1"/>
-    <col min="4" max="7" width="17.1796875" style="98" customWidth="1"/>
-    <col min="8" max="12" width="12.81640625" style="98" customWidth="1"/>
-    <col min="13" max="16384" width="12.81640625" style="98"/>
+    <col min="2" max="2" width="27.44140625" style="98" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="98" customWidth="1"/>
+    <col min="4" max="7" width="17.21875" style="98" customWidth="1"/>
+    <col min="8" max="12" width="12.77734375" style="98" customWidth="1"/>
+    <col min="13" max="16384" width="12.77734375" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
         <v>163</v>
       </c>
@@ -32435,12 +32439,12 @@
       </c>
       <c r="H7" s="79"/>
     </row>
-    <row r="9" spans="1:8" s="89" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="71" t="s">
         <v>163</v>
       </c>
@@ -32605,12 +32609,12 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="89" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="89" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="89" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="71" t="s">
         <v>163</v>
       </c>
@@ -32792,14 +32796,14 @@
       <selection activeCell="C11" activeCellId="2" sqref="C35 C23:F23 C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" customWidth="1"/>
-    <col min="2" max="2" width="31.36328125" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
     <col min="3" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="str">
         <f>"Porcentaje de muertes en el año de referencia ("&amp;start_year&amp;") atribuible a la causa"</f>
         <v>Porcentaje de muertes en el año de referencia (2021) atribuible a la causa</v>
@@ -32810,7 +32814,7 @@
       <c r="E1" s="20"/>
       <c r="F1" s="20"/>
     </row>
-    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -32877,7 +32881,7 @@
       <c r="B11" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="103">
+      <c r="C11" s="101">
         <f>SUM(C3:C10)</f>
         <v>0</v>
       </c>
@@ -32893,7 +32897,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="98" t="s">
         <v>83</v>
       </c>
@@ -32999,19 +33003,19 @@
       <c r="B23" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="103">
+      <c r="C23" s="101">
         <f>SUM(C14:C22)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="103">
+      <c r="D23" s="101">
         <f>SUM(D14:D22)</f>
         <v>0</v>
       </c>
-      <c r="E23" s="103">
+      <c r="E23" s="101">
         <f>SUM(E14:E22)</f>
         <v>0</v>
       </c>
-      <c r="F23" s="103">
+      <c r="F23" s="101">
         <f>SUM(F14:F22)</f>
         <v>0</v>
       </c>
@@ -33027,7 +33031,7 @@
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -33101,7 +33105,7 @@
       <c r="B35" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="103">
+      <c r="C35" s="101">
         <f>SUM(C26:C34)</f>
         <v>0</v>
       </c>
@@ -33124,13 +33128,13 @@
       <selection activeCell="C15" activeCellId="2" sqref="C2:G3 C8:G9 C15:O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="str">
         <f>"Porcentaje de población en cada categoría en el año de referencia ("&amp;start_year&amp;")"</f>
         <v>Porcentaje de población en cada categoría en el año de referencia (2021)</v>
@@ -33161,23 +33165,23 @@
       <c r="B2" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="104" t="str">
+      <c r="C2" s="102" t="str">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE), "")</f>
         <v/>
       </c>
-      <c r="D2" s="104" t="str">
+      <c r="D2" s="102" t="str">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE), "")</f>
         <v/>
       </c>
-      <c r="E2" s="104" t="str">
+      <c r="E2" s="102" t="str">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE), "")</f>
         <v/>
       </c>
-      <c r="F2" s="104" t="str">
+      <c r="F2" s="102" t="str">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE), "")</f>
         <v/>
       </c>
-      <c r="G2" s="104" t="str">
+      <c r="G2" s="102" t="str">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE), "")</f>
         <v/>
       </c>
@@ -33186,23 +33190,23 @@
       <c r="B3" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="104" t="str">
+      <c r="C3" s="102" t="str">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
         <v/>
       </c>
-      <c r="D3" s="104" t="str">
+      <c r="D3" s="102" t="str">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5), "")</f>
         <v/>
       </c>
-      <c r="E3" s="104" t="str">
+      <c r="E3" s="102" t="str">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - SUM(E4:E5), "")</f>
         <v/>
       </c>
-      <c r="F3" s="104" t="str">
+      <c r="F3" s="102" t="str">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - SUM(F4:F5), "")</f>
         <v/>
       </c>
-      <c r="G3" s="104" t="str">
+      <c r="G3" s="102" t="str">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - SUM(G4:G5), "")</f>
         <v/>
       </c>
@@ -33250,23 +33254,23 @@
       <c r="B8" s="70" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="104" t="str">
+      <c r="C8" s="102" t="str">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE), "")</f>
         <v/>
       </c>
-      <c r="D8" s="104" t="str">
+      <c r="D8" s="102" t="str">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE), "")</f>
         <v/>
       </c>
-      <c r="E8" s="104" t="str">
+      <c r="E8" s="102" t="str">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE), "")</f>
         <v/>
       </c>
-      <c r="F8" s="104" t="str">
+      <c r="F8" s="102" t="str">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE), "")</f>
         <v/>
       </c>
-      <c r="G8" s="104" t="str">
+      <c r="G8" s="102" t="str">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE), "")</f>
         <v/>
       </c>
@@ -33275,23 +33279,23 @@
       <c r="B9" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="104" t="str">
+      <c r="C9" s="102" t="str">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
         <v/>
       </c>
-      <c r="D9" s="104" t="str">
+      <c r="D9" s="102" t="str">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11), "")</f>
         <v/>
       </c>
-      <c r="E9" s="104" t="str">
+      <c r="E9" s="102" t="str">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - SUM(E10:E11), "")</f>
         <v/>
       </c>
-      <c r="F9" s="104" t="str">
+      <c r="F9" s="102" t="str">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - SUM(F10:F11), "")</f>
         <v/>
       </c>
-      <c r="G9" s="104" t="str">
+      <c r="G9" s="102" t="str">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - SUM(G10:G11), "")</f>
         <v/>
       </c>
@@ -33396,55 +33400,55 @@
       <c r="B15" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="C15" s="104">
+      <c r="C15" s="102">
         <f t="shared" ref="C15:O15" si="0">iron_deficiency_anaemia*C14</f>
         <v>0</v>
       </c>
-      <c r="D15" s="104">
+      <c r="D15" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E15" s="104">
+      <c r="E15" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F15" s="104">
+      <c r="F15" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="104">
+      <c r="G15" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H15" s="104">
+      <c r="H15" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="104">
+      <c r="I15" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="104">
+      <c r="J15" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K15" s="104">
+      <c r="K15" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L15" s="104">
+      <c r="L15" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M15" s="104">
+      <c r="M15" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N15" s="104">
+      <c r="N15" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O15" s="104">
+      <c r="O15" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -33481,13 +33485,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.90625" customWidth="1"/>
-    <col min="2" max="7" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
+    <col min="2" max="7" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="str">
         <f>"Porcentaje de niños en cada categoría en el año de referencia ("&amp;start_year&amp;")"</f>
         <v>Porcentaje de niños en cada categoría en el año de referencia (2021)</v>
@@ -33548,23 +33552,23 @@
       <c r="B5" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="104">
+      <c r="C5" s="102">
         <f>1-C2-C3-C4</f>
         <v>1</v>
       </c>
-      <c r="D5" s="104">
+      <c r="D5" s="102">
         <f t="shared" ref="D5:G5" si="0">1-D2-D3-D4</f>
         <v>1</v>
       </c>
-      <c r="E5" s="104">
+      <c r="E5" s="102">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F5" s="104">
+      <c r="F5" s="102">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G5" s="104">
+      <c r="G5" s="102">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -33587,13 +33591,13 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>135</v>
       </c>
@@ -33813,13 +33817,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>147</v>
       </c>
@@ -33889,19 +33893,19 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D19" sqref="D19:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="98" customWidth="1"/>
-    <col min="2" max="2" width="19.08984375" style="98" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="98" customWidth="1"/>
-    <col min="4" max="8" width="11.453125" style="98" customWidth="1"/>
-    <col min="9" max="16384" width="11.453125" style="98"/>
+    <col min="2" max="2" width="19.109375" style="98" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="98" customWidth="1"/>
+    <col min="4" max="8" width="11.44140625" style="98" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>154</v>
       </c>
@@ -33918,7 +33922,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>151</v>
       </c>
@@ -33936,8 +33940,8 @@
       <c r="B3" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="43" t="b">
-        <v>1</v>
+      <c r="C3" s="43" t="s">
+        <v>5</v>
       </c>
       <c r="D3" s="43"/>
       <c r="E3" s="28" t="str">
@@ -33949,8 +33953,8 @@
       <c r="B4" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="43" t="b">
-        <v>1</v>
+      <c r="C4" s="43" t="s">
+        <v>5</v>
       </c>
       <c r="D4" s="43"/>
       <c r="E4" s="28" t="str">
@@ -33962,8 +33966,8 @@
       <c r="B5" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="43" t="b">
-        <v>1</v>
+      <c r="C5" s="43" t="s">
+        <v>5</v>
       </c>
       <c r="D5" s="43"/>
       <c r="E5" s="28" t="str">
@@ -33975,8 +33979,8 @@
       <c r="B6" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="43" t="b">
-        <v>1</v>
+      <c r="C6" s="43" t="s">
+        <v>5</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="28" t="str">
@@ -33992,7 +33996,7 @@
       <c r="D7" s="21"/>
       <c r="E7" s="43"/>
     </row>
-    <row r="9" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>152</v>
       </c>
@@ -34000,9 +34004,7 @@
         <v>104</v>
       </c>
       <c r="C9" s="43"/>
-      <c r="D9" s="43" t="b">
-        <v>0</v>
-      </c>
+      <c r="D9" s="43"/>
       <c r="E9" s="28" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -34013,7 +34015,9 @@
         <v>78</v>
       </c>
       <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
+      <c r="D10" s="43" t="s">
+        <v>5</v>
+      </c>
       <c r="E10" s="28" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -34024,7 +34028,9 @@
         <v>74</v>
       </c>
       <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
+      <c r="D11" s="43" t="s">
+        <v>5</v>
+      </c>
       <c r="E11" s="28" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -34035,7 +34041,9 @@
         <v>77</v>
       </c>
       <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
+      <c r="D12" s="43" t="s">
+        <v>5</v>
+      </c>
       <c r="E12" s="28" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -34046,7 +34054,9 @@
         <v>75</v>
       </c>
       <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
+      <c r="D13" s="43" t="s">
+        <v>5</v>
+      </c>
       <c r="E13" s="28" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -34058,11 +34068,9 @@
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="21"/>
-      <c r="E14" s="43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="E14" s="43"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>153</v>
       </c>
@@ -34070,9 +34078,7 @@
         <v>104</v>
       </c>
       <c r="C16" s="43"/>
-      <c r="D16" s="43" t="s">
-        <v>5</v>
-      </c>
+      <c r="D16" s="43"/>
       <c r="E16" s="28" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -34109,9 +34115,7 @@
         <v>77</v>
       </c>
       <c r="C19" s="43"/>
-      <c r="D19" s="43" t="s">
-        <v>5</v>
-      </c>
+      <c r="D19" s="43"/>
       <c r="E19" s="28" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -34122,9 +34126,7 @@
         <v>75</v>
       </c>
       <c r="C20" s="43"/>
-      <c r="D20" s="43" t="s">
-        <v>5</v>
-      </c>
+      <c r="D20" s="43"/>
       <c r="E20" s="28" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -34156,15 +34158,15 @@
       <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
@@ -34178,7 +34180,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>163</v>
       </c>
@@ -34190,7 +34192,7 @@
       </c>
       <c r="D2" s="43"/>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>160</v>
       </c>

</xml_diff>